<commit_message>
update datasets: adjectivalness dataset cleanup
</commit_message>
<xml_diff>
--- a/adjectivalness_analysis.xlsx
+++ b/adjectivalness_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_envs\Adjectivalness_PennTreebank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/julie_nijs_kuleuven_be/Documents/keep_Ving/keep_V-ing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A96F43-C05A-42E9-8B75-5B596C9FDB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F0A96F43-C05A-42E9-8B75-5B596C9FDB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A9E0881-A6F0-4FAA-B870-BD4ABDBD1159}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,13 +452,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,13 +484,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,18 +795,19 @@
   <dimension ref="A1:D126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,721 +821,721 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>4</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>74</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>35</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0.47297297297297303</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>9</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>4</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>5</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>10</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>4</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>20</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>8</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>11</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>4</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>0.36363636363636359</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>108</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>38</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>0.35185185185185192</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>66</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>22</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>3</v>
       </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>3</v>
       </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>3</v>
       </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>6</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>2</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>26</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>8</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>0.30769230769230771</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>221</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>67</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>0.30316742081447962</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>194</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>54</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>0.27835051546391748</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>12</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>3</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>29</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>7</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>0.2413793103448276</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>9</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>2</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>37</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>7</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>0.1891891891891892</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>48</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>9</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>0.1875</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>11</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>2</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>0.1818181818181818</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>17</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>3</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>0.1764705882352941</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>23</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>4</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>0.17391304347826089</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>36</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>6</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>0.16666666666666671</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>44</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>7</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>0.15909090909090909</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>151</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>24</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>0.15894039735099341</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>13</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>2</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>0.15384615384615391</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>72</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>11</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>0.15277777777777779</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>67</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>10</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>0.1492537313432836</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>76</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>11</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>0.14473684210526319</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>49</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>7</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>7</v>
       </c>
-      <c r="C44" s="3">
-        <v>1</v>
-      </c>
-      <c r="D44" s="3">
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2">
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>21</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>3</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>7</v>
       </c>
-      <c r="C46" s="3">
-        <v>1</v>
-      </c>
-      <c r="D46" s="3">
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2">
         <v>0.14285714285714279</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>16</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>2</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>0.125</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>24</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>3</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>0.125</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>8</v>
       </c>
-      <c r="C49" s="3">
-        <v>1</v>
-      </c>
-      <c r="D49" s="3">
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
         <v>0.125</v>
       </c>
     </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>8</v>
       </c>
-      <c r="C50" s="3">
-        <v>1</v>
-      </c>
-      <c r="D50" s="3">
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
         <v>0.125</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>255</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>30</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>0.1176470588235294</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>43</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>5</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>0.1162790697674419</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
@@ -1555,1025 +1549,1025 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="2">
         <v>114</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="2">
         <v>11</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="2">
         <v>9.6491228070175433E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="2">
         <v>141</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>13</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="2">
         <v>9.2198581560283682E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="2">
         <v>11</v>
       </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="2">
         <v>11</v>
       </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57">
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2">
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="2">
         <v>123</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>11</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="2">
         <v>8.943089430894309E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="2">
         <v>24</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>2</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="2">
         <v>174</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="2">
         <v>14</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="2">
         <v>8.0459770114942528E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="2">
         <v>101</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="2">
         <v>8</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="2">
         <v>7.9207920792079209E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="2">
         <v>279</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="2">
         <v>20</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="2">
         <v>7.1684587813620068E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="2">
         <v>14</v>
       </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="2">
         <v>117</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="2">
         <v>8</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="2">
         <v>6.8376068376068383E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="2">
         <v>15</v>
       </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65">
+      <c r="C65" s="2">
+        <v>1</v>
+      </c>
+      <c r="D65" s="2">
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="2">
         <v>60</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="2">
         <v>4</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="2">
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="2">
         <v>16</v>
       </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="2">
         <v>52</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="2">
         <v>3</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="2">
         <v>5.7692307692307702E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="2">
         <v>18</v>
       </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69">
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2">
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="2">
         <v>75</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="2">
         <v>4</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="2">
         <v>5.3333333333333337E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="2">
         <v>45</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="2">
         <v>2</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="2">
         <v>4.4444444444444453E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="2">
         <v>23</v>
       </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
+      <c r="C72" s="2">
+        <v>1</v>
+      </c>
+      <c r="D72" s="2">
         <v>4.3478260869565223E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="2">
         <v>110</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="2">
         <v>4</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="2">
         <v>3.6363636363636362E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="2">
         <v>28</v>
       </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-      <c r="D74">
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74" s="2">
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="2">
         <v>76</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="2">
         <v>2</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="2">
         <v>2.6315789473684209E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="2">
         <v>173</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="2">
         <v>4</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="2">
         <v>2.312138728323699E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="2">
         <v>100</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="2">
         <v>2</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="2">
         <v>0.02</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="2">
         <v>163</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="2">
         <v>2</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="2">
         <v>1.226993865030675E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="2">
         <v>712</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="2">
         <v>7</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="2">
         <v>9.8314606741573031E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="2">
         <v>113</v>
       </c>
-      <c r="C80">
-        <v>1</v>
-      </c>
-      <c r="D80">
+      <c r="C80" s="2">
+        <v>1</v>
+      </c>
+      <c r="D80" s="2">
         <v>8.8495575221238937E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="2">
         <v>145</v>
       </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-      <c r="D81">
+      <c r="C81" s="2">
+        <v>1</v>
+      </c>
+      <c r="D81" s="2">
         <v>6.8965517241379309E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="2">
         <v>399</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="2">
         <v>2</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="2">
         <v>5.0125313283208017E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B83">
-        <v>0</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B83" s="2">
+        <v>0</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="2">
         <v>13</v>
       </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="C84" s="2">
+        <v>0</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B85">
-        <v>0</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="B85" s="2">
+        <v>0</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="B86" s="2">
+        <v>0</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="2">
         <v>2</v>
       </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-      <c r="D87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="C87" s="2">
+        <v>0</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B88">
-        <v>0</v>
-      </c>
-      <c r="C88">
-        <v>0</v>
-      </c>
-      <c r="D88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="B88" s="2">
+        <v>0</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0</v>
+      </c>
+      <c r="D88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
-      <c r="C89">
-        <v>0</v>
-      </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="B89" s="2">
+        <v>1</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B90">
-        <v>0</v>
-      </c>
-      <c r="C90">
-        <v>0</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B90" s="2">
+        <v>0</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="2">
         <v>5</v>
       </c>
-      <c r="C91">
-        <v>0</v>
-      </c>
-      <c r="D91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="C91" s="2">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="2">
         <v>32</v>
       </c>
-      <c r="C92">
-        <v>0</v>
-      </c>
-      <c r="D92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="C92" s="2">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="2">
         <v>7</v>
       </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="C93" s="2">
+        <v>0</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="2">
         <v>7</v>
       </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="C94" s="2">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="2">
         <v>3</v>
       </c>
-      <c r="C95">
-        <v>0</v>
-      </c>
-      <c r="D95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="C95" s="2">
+        <v>0</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B96">
-        <v>0</v>
-      </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="B96" s="2">
+        <v>0</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-      <c r="C97">
-        <v>0</v>
-      </c>
-      <c r="D97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="B97" s="2">
+        <v>1</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B98">
-        <v>1</v>
-      </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="B98" s="2">
+        <v>1</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B99">
-        <v>1</v>
-      </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-      <c r="D99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="B99" s="2">
+        <v>1</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B100">
-        <v>0</v>
-      </c>
-      <c r="C100">
-        <v>0</v>
-      </c>
-      <c r="D100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="B100" s="2">
+        <v>0</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-      <c r="C101">
-        <v>0</v>
-      </c>
-      <c r="D101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="B101" s="2">
+        <v>1</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="2">
         <v>4</v>
       </c>
-      <c r="C102">
-        <v>0</v>
-      </c>
-      <c r="D102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="C102" s="2">
+        <v>0</v>
+      </c>
+      <c r="D102" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B103">
-        <v>0</v>
-      </c>
-      <c r="C103">
-        <v>0</v>
-      </c>
-      <c r="D103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="B103" s="2">
+        <v>0</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="2">
         <v>5</v>
       </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-      <c r="D104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="C104" s="2">
+        <v>0</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B105">
-        <v>0</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="B105" s="2">
+        <v>0</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B106">
-        <v>1</v>
-      </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="B106" s="2">
+        <v>1</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0</v>
+      </c>
+      <c r="D106" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="2">
         <v>10</v>
       </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-      <c r="D107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="C107" s="2">
+        <v>0</v>
+      </c>
+      <c r="D107" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="2">
         <v>2</v>
       </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
-      <c r="D108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="C108" s="2">
+        <v>0</v>
+      </c>
+      <c r="D108" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="2">
         <v>4</v>
       </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="C109" s="2">
+        <v>0</v>
+      </c>
+      <c r="D109" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B110">
-        <v>1</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="B110" s="2">
+        <v>1</v>
+      </c>
+      <c r="C110" s="2">
+        <v>0</v>
+      </c>
+      <c r="D110" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B111">
-        <v>0</v>
-      </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-      <c r="D111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="B111" s="2">
+        <v>0</v>
+      </c>
+      <c r="C111" s="2">
+        <v>0</v>
+      </c>
+      <c r="D111" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="2">
         <v>26</v>
       </c>
-      <c r="C112">
-        <v>0</v>
-      </c>
-      <c r="D112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="C112" s="2">
+        <v>0</v>
+      </c>
+      <c r="D112" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B113">
-        <v>0</v>
-      </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
-      <c r="D113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="B113" s="2">
+        <v>0</v>
+      </c>
+      <c r="C113" s="2">
+        <v>0</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="2">
         <v>3</v>
       </c>
-      <c r="C114">
-        <v>0</v>
-      </c>
-      <c r="D114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="C114" s="2">
+        <v>0</v>
+      </c>
+      <c r="D114" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B115">
-        <v>1</v>
-      </c>
-      <c r="C115">
-        <v>0</v>
-      </c>
-      <c r="D115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B115" s="2">
+        <v>1</v>
+      </c>
+      <c r="C115" s="2">
+        <v>0</v>
+      </c>
+      <c r="D115" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B116">
-        <v>0</v>
-      </c>
-      <c r="C116">
-        <v>0</v>
-      </c>
-      <c r="D116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="B116" s="2">
+        <v>0</v>
+      </c>
+      <c r="C116" s="2">
+        <v>0</v>
+      </c>
+      <c r="D116" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B117">
-        <v>1</v>
-      </c>
-      <c r="C117">
-        <v>0</v>
-      </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="B117" s="2">
+        <v>1</v>
+      </c>
+      <c r="C117" s="2">
+        <v>0</v>
+      </c>
+      <c r="D117" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="2">
         <v>5</v>
       </c>
-      <c r="C118">
-        <v>0</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="C118" s="2">
+        <v>0</v>
+      </c>
+      <c r="D118" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B119">
-        <v>0</v>
-      </c>
-      <c r="C119">
-        <v>0</v>
-      </c>
-      <c r="D119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="B119" s="2">
+        <v>0</v>
+      </c>
+      <c r="C119" s="2">
+        <v>0</v>
+      </c>
+      <c r="D119" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="2">
         <v>8</v>
       </c>
-      <c r="C120">
-        <v>0</v>
-      </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+      <c r="C120" s="2">
+        <v>0</v>
+      </c>
+      <c r="D120" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="2">
         <v>4</v>
       </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+      <c r="C121" s="2">
+        <v>0</v>
+      </c>
+      <c r="D121" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="2">
         <v>12</v>
       </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="C122" s="2">
+        <v>0</v>
+      </c>
+      <c r="D122" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="2">
         <v>4</v>
       </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
-      <c r="D123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+      <c r="C123" s="2">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B124">
-        <v>0</v>
-      </c>
-      <c r="C124">
-        <v>0</v>
-      </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+      <c r="B124" s="2">
+        <v>0</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="2">
         <v>16</v>
       </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
-      <c r="D125">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="C125" s="2">
+        <v>0</v>
+      </c>
+      <c r="D125" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="2">
         <v>21</v>
       </c>
-      <c r="C126">
-        <v>0</v>
-      </c>
-      <c r="D126">
+      <c r="C126" s="2">
+        <v>0</v>
+      </c>
+      <c r="D126" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>